<commit_message>
reformat after sheet cleanup
</commit_message>
<xml_diff>
--- a/rules/CORE-000598/negative/01/data/unit-test-coreid-CG0413-negative.xlsx
+++ b/rules/CORE-000598/negative/01/data/unit-test-coreid-CG0413-negative.xlsx
@@ -1,99 +1,66 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
   <sheets>
-    <sheet name="Datasets" sheetId="1" r:id="rId1"/>
-    <sheet name="alb.xpt" sheetId="2" r:id="rId2"/>
+    <sheet name="Datasets" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="alb.xpt" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Validation" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <i val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <i/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none">
-        <bgColor/>
-      </patternFill>
+      <patternFill/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -102,23 +69,88 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs>
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="1" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -197,7 +229,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -232,7 +263,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -267,16 +297,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -398,205 +432,258 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="str">
-        <v>Filename</v>
-      </c>
-      <c r="B1" s="3" t="str">
-        <v>Label</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Label</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="str">
-        <v>alb.xpt</v>
-      </c>
-      <c r="B2" s="4" t="str">
-        <v>Laboratory Test Results A</v>
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>alb.xpt</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Laboratory Test Results A</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
-  </ignoredErrors>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="str">
-        <v>STUDYID</v>
-      </c>
-      <c r="B1" s="5" t="str">
-        <v>DOMAIN</v>
-      </c>
-      <c r="C1" s="5" t="str">
-        <v>USUBJID</v>
-      </c>
-      <c r="D1" s="5" t="str">
-        <v>LBTESTCD</v>
-      </c>
-      <c r="E1" s="5" t="str">
-        <v>LBTEST</v>
-      </c>
-      <c r="F1" s="5" t="str">
-        <v>LBSTREFC</v>
-      </c>
-      <c r="G1" s="5" t="str">
-        <v>LBSTREFN</v>
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>STUDYID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>DOMAIN</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>USUBJID</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>LBTESTCD</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>LBTEST</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>LBSTREFC</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>LBSTREFN</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="str">
-        <v>Study Identifier</v>
-      </c>
-      <c r="B2" s="5" t="str">
-        <v>Domain Abbreviation</v>
-      </c>
-      <c r="C2" s="5" t="str">
-        <v>Unique Subject Identifier</v>
-      </c>
-      <c r="D2" s="6" t="str">
-        <v>Lab Test or Examination Short Name</v>
-      </c>
-      <c r="E2" s="6" t="str">
-        <v>Lab Test or Examination Name</v>
-      </c>
-      <c r="F2" s="5" t="str">
-        <v>Character Reference Result</v>
-      </c>
-      <c r="G2" s="5" t="str">
-        <v>Numeric Reference Result in Std Units</v>
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>Study Identifier</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Domain Abbreviation</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Unique Subject Identifier</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>Lab Test or Examination Short Name</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>Lab Test or Examination Name</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>Character Reference Result</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>Numeric Reference Result in Std Units</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>Char</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v>Char</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>Char</v>
-      </c>
-      <c r="D3" s="6" t="str">
-        <v>Char</v>
-      </c>
-      <c r="E3" s="6" t="str">
-        <v>Char</v>
-      </c>
-      <c r="F3" s="5" t="str">
-        <v>Char</v>
-      </c>
-      <c r="G3" s="5" t="str">
-        <v>Num</v>
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Char</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Char</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>Char</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>Char</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>Char</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>Char</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>Num</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5">
+      <c r="A4" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>CDISCPILOT01</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>LB</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>CDISC001</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E5" s="5" t="str">
-        <v/>
-      </c>
-      <c r="F5" s="5" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="G5" s="5" t="str">
-        <v>8</v>
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>CDISCPILOT01</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>LB</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>CDISC001</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="n"/>
+      <c r="E5" s="3" t="n"/>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G5"/>
-  </ignoredErrors>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Sheet</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>